<commit_message>
Initial unit_test for CoreModel
</commit_message>
<xml_diff>
--- a/mario/test/IOT_dummy.xlsx
+++ b/mario/test/IOT_dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/MARIO/mario/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10460172-1749-CE46-BDEC-F12B911228D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10128AC3-0094-2245-9C73-1CF28C8968EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" firstSheet="2" activeTab="17" xr2:uid="{CEC85D7C-5B4B-894B-A949-5EF332C1C6B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" firstSheet="4" activeTab="18" xr2:uid="{CEC85D7C-5B4B-894B-A949-5EF332C1C6B0}"/>
   </bookViews>
   <sheets>
     <sheet name="all_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,8 @@
     <sheet name="F" sheetId="17" r:id="rId16"/>
     <sheet name="_m" sheetId="18" r:id="rId17"/>
     <sheet name="M" sheetId="19" r:id="rId18"/>
-    <sheet name="usefull" sheetId="12" r:id="rId19"/>
+    <sheet name="units" sheetId="20" r:id="rId19"/>
+    <sheet name="usefull" sheetId="12" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="24">
   <si>
     <t>reg1</t>
   </si>
@@ -107,6 +108,24 @@
   </si>
   <si>
     <t>Y_total</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>eur</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Factor of production</t>
+  </si>
+  <si>
+    <t>Satellite account</t>
   </si>
 </sst>
 </file>
@@ -477,7 +496,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1765,7 +1784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C4C3EE-6C05-FF42-9A36-F65EA63B30E6}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1854,141 +1873,106 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E5E29-E0F3-EE4E-B920-A0460F875ECA}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAE65AB-EAB4-474B-B367-27AB37CA61C5}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <f>SUM(_v!B4:B5)</f>
-        <v>0.78902953586497881</v>
-      </c>
-      <c r="C4">
-        <f>SUM(_v!C4:C5)</f>
-        <v>0.76956521739130435</v>
-      </c>
-      <c r="D4">
-        <f>SUM(_v!D4:D5)</f>
-        <v>0.73026315789473673</v>
-      </c>
-      <c r="E4">
-        <f>SUM(_v!E4:E5)</f>
-        <v>0.85673352435530081</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <f>SUM(Y!D4:G4)</f>
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <f>SUM(Y!D5:G5)</f>
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <f>SUM(Y!D6:G6)</f>
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <f>SUM(Y!D7:G7)</f>
-        <v>271</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2088,6 +2072,149 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E5E29-E0F3-EE4E-B920-A0460F875ECA}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f>SUM(_v!B4:B5)</f>
+        <v>0.78902953586497881</v>
+      </c>
+      <c r="C4">
+        <f>SUM(_v!C4:C5)</f>
+        <v>0.76956521739130435</v>
+      </c>
+      <c r="D4">
+        <f>SUM(_v!D4:D5)</f>
+        <v>0.73026315789473673</v>
+      </c>
+      <c r="E4">
+        <f>SUM(_v!E4:E5)</f>
+        <v>0.85673352435530081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f>SUM(Y!D4:G4)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>SUM(Y!D5:G5)</f>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f>SUM(Y!D6:G6)</f>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f>SUM(Y!D7:G7)</f>
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5946CB-045A-6947-8800-8FD8EBA15667}">
   <dimension ref="A1:E5"/>
@@ -2185,7 +2312,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>